<commit_message>
feat: change inter to international in plo template
</commit_message>
<xml_diff>
--- a/public/template/plo.xlsx
+++ b/public/template/plo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puntf\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\inu-garden\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DECD71-C4CB-47CA-9CC4-A5AE0DF0221A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E7E9A0-010A-48BD-8DB9-8B8674200159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLO" sheetId="1" r:id="rId1"/>
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -506,7 +506,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{644D5A9C-A6DB-474B-B803-91611F4F8D25}">
-      <formula1>"regular,inter"</formula1>
+      <formula1>"regular,international"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46770CF-0A86-4130-9EA2-CFBA896C7198}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>